<commit_message>
ft: edited invoke for az
</commit_message>
<xml_diff>
--- a/data/azerbaijan_8.xlsx
+++ b/data/azerbaijan_8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fdduarte/Development/universidad/tesis/calendar-opt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E6B0F5-CCAF-3347-9EAD-5C69859F8E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275D4E6A-9D6D-DD47-B2FE-81AAC151FE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="43">
   <si>
     <t>Jornada</t>
   </si>
@@ -142,6 +142,30 @@
   </si>
   <si>
     <t>Puntos al finalizar la primera rueda</t>
+  </si>
+  <si>
+    <t>QAR</t>
+  </si>
+  <si>
+    <t>GAB</t>
+  </si>
+  <si>
+    <t>ZIR</t>
+  </si>
+  <si>
+    <t>NEF</t>
+  </si>
+  <si>
+    <t>SAB</t>
+  </si>
+  <si>
+    <t>SAM</t>
+  </si>
+  <si>
+    <t>SUM</t>
+  </si>
+  <si>
+    <t>SEB</t>
   </si>
 </sst>
 </file>
@@ -551,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -588,43 +612,52 @@
         <v>44702</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="2">
+        <v>44702</v>
+      </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B5" s="2">
+        <v>44702</v>
+      </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="2">
+        <v>44702</v>
+      </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
@@ -637,46 +670,55 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
-        <v>44696</v>
+        <v>44702</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
+        <v>44702</v>
+      </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="2">
+        <v>44702</v>
+      </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="2">
+        <v>44702</v>
+      </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E11" t="s">
         <v>27</v>
@@ -689,24 +731,27 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
-        <v>44689</v>
+        <v>44702</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="2">
+        <v>44702</v>
+      </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="E14" t="s">
         <v>23</v>
@@ -714,24 +759,27 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
-        <v>44690</v>
+        <v>44702</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D15" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="2">
+        <v>44702</v>
+      </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
         <v>21</v>
@@ -744,24 +792,27 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
-        <v>44684</v>
+        <v>44702</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="E18" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="2">
+        <v>44702</v>
+      </c>
       <c r="C19" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
         <v>15</v>
@@ -769,24 +820,27 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
-        <v>44685</v>
+        <v>44702</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E20" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="2">
+        <v>44702</v>
+      </c>
       <c r="C21" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E21" t="s">
         <v>14</v>
@@ -799,46 +853,55 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
-        <v>44675</v>
+        <v>44702</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="2">
+        <v>44702</v>
+      </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D24" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="E24" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="2">
+        <v>44702</v>
+      </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E25" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="2">
+        <v>44702</v>
+      </c>
       <c r="C26" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="E26" t="s">
         <v>13</v>
@@ -851,24 +914,27 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
-        <v>44666</v>
+        <v>44702</v>
       </c>
       <c r="C28" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D28" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E28" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="2">
+        <v>44702</v>
+      </c>
       <c r="C29" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="E29" t="s">
         <v>29</v>
@@ -876,24 +942,27 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" s="2">
-        <v>44667</v>
+        <v>44702</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="E30" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="2">
+        <v>44702</v>
+      </c>
       <c r="C31" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D31" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E31" t="s">
         <v>21</v>
@@ -906,24 +975,27 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" s="2">
-        <v>44660</v>
+        <v>44702</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="2">
+        <v>44702</v>
+      </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="E34" t="s">
         <v>24</v>
@@ -931,24 +1003,27 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B35" s="2">
-        <v>44661</v>
+        <v>44702</v>
       </c>
       <c r="C35" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D35" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E35" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="2">
+        <v>44702</v>
+      </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E36" t="s">
         <v>20</v>
@@ -961,24 +1036,27 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B38" s="2">
-        <v>44653</v>
+        <v>44702</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="E38" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B39" s="2">
+        <v>44702</v>
+      </c>
       <c r="C39" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D39" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E39" t="s">
         <v>27</v>
@@ -986,24 +1064,27 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B40" s="2">
-        <v>44654</v>
+        <v>44702</v>
       </c>
       <c r="C40" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="E40" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B41" s="2">
+        <v>44702</v>
+      </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="E41" t="s">
         <v>15</v>
@@ -1016,24 +1097,27 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B43" s="2">
-        <v>44638</v>
+        <v>44702</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E43" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="2">
+        <v>44702</v>
+      </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E44" t="s">
         <v>25</v>
@@ -1041,24 +1125,27 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B45" s="2">
-        <v>44639</v>
+        <v>44702</v>
       </c>
       <c r="C45" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="E45" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B46" s="2">
+        <v>44702</v>
+      </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D46" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E46" t="s">
         <v>27</v>
@@ -1071,24 +1158,27 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B48" s="2">
-        <v>44632</v>
+        <v>44702</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="E48" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B49" s="2">
+        <v>44702</v>
+      </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D49" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E49" t="s">
         <v>13</v>
@@ -1096,13 +1186,13 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B50" s="2">
-        <v>44633</v>
+        <v>44702</v>
       </c>
       <c r="C50" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E50" t="s">
         <v>19</v>
@@ -1110,13 +1200,13 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B51" s="2">
-        <v>44634</v>
+        <v>44702</v>
       </c>
       <c r="C51" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D51" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="E51" t="s">
         <v>23</v>
@@ -1129,24 +1219,27 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B53" s="2">
-        <v>44625</v>
+        <v>44702</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D53" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E53" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B54" s="2">
+        <v>44702</v>
+      </c>
       <c r="C54" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D54" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="E54" t="s">
         <v>18</v>
@@ -1154,24 +1247,27 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B55" s="2">
-        <v>44626</v>
+        <v>44702</v>
       </c>
       <c r="C55" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D55" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E55" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="2">
+        <v>44702</v>
+      </c>
       <c r="C56" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E56" t="s">
         <v>28</v>
@@ -1184,24 +1280,27 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B58" s="2">
-        <v>44619</v>
+        <v>44702</v>
       </c>
       <c r="C58" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E58" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B59" s="2">
+        <v>44702</v>
+      </c>
       <c r="C59" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D59" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E59" t="s">
         <v>26</v>
@@ -1209,24 +1308,27 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B60" s="2">
-        <v>44620</v>
+        <v>44702</v>
       </c>
       <c r="C60" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D60" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="E60" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B61" s="2">
+        <v>44702</v>
+      </c>
       <c r="C61" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D61" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E61" t="s">
         <v>23</v>
@@ -1239,24 +1341,27 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B63" s="2">
-        <v>44611</v>
+        <v>44702</v>
       </c>
       <c r="C63" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D63" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="E63" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B64" s="2">
+        <v>44702</v>
+      </c>
       <c r="C64" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D64" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="E64" t="s">
         <v>24</v>
@@ -1264,13 +1369,13 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B65" s="2">
-        <v>44612</v>
+        <v>44702</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D65" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="E65" t="s">
         <v>18</v>
@@ -1278,13 +1383,13 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B66" s="2">
-        <v>44693</v>
+        <v>44702</v>
       </c>
       <c r="C66" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D66" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E66" t="s">
         <v>22</v>
@@ -1297,24 +1402,27 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B68" s="2">
-        <v>44599</v>
+        <v>44702</v>
       </c>
       <c r="C68" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D68" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="E68" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B69" s="2">
+        <v>44702</v>
+      </c>
       <c r="C69" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D69" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="E69" t="s">
         <v>19</v>
@@ -1322,24 +1430,27 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B70" s="2">
-        <v>44600</v>
+        <v>44702</v>
       </c>
       <c r="C70" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D70" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="E70" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B71" s="2">
+        <v>44702</v>
+      </c>
       <c r="C71" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D71" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="E71" t="s">
         <v>15</v>
@@ -1455,7 +1566,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1486,7 +1597,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <f>33+16</f>
@@ -1505,7 +1616,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <f>26+8</f>
@@ -1524,7 +1635,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <f>22+11</f>
@@ -1543,7 +1654,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <f>22+16</f>
@@ -1562,7 +1673,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <f>17+6</f>
@@ -1581,7 +1692,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D7">
         <f>14+9</f>
@@ -1600,7 +1711,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="D8">
         <f>12+1</f>
@@ -1619,7 +1730,7 @@
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <f>10+0</f>

</xml_diff>